<commit_message>
pH assay output update
</commit_message>
<xml_diff>
--- a/output/20230503_4NP_butyrate_p55_pH_slope_differences_combined.xlsx
+++ b/output/20230503_4NP_butyrate_p55_pH_slope_differences_combined.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,23 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robinsse/Documents/github/platereader-plotting/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2CC3B2B1-8C2A-F147-8518-765924370338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D25A5EE-33CD-4D48-8235-091E86A6DBA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3980" yWindow="500" windowWidth="31800" windowHeight="18240"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="20230503_4NP_butyrate_p55_pH_sl" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'20230503_4NP_butyrate_p55_pH_sl'!$G$2:$G$7</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'20230503_4NP_butyrate_p55_pH_sl'!$H$2:$H$7</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'20230503_4NP_butyrate_p55_pH_sl'!$G$2:$G$7</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'20230503_4NP_butyrate_p55_pH_sl'!$H$2:$H$7</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'20230503_4NP_butyrate_p55_pH_sl'!$G$2:$G$7</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'20230503_4NP_butyrate_p55_pH_sl'!$H$2:$H$7</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'20230503_4NP_butyrate_p55_pH_sl'!$G$2:$G$7</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'20230503_4NP_butyrate_p55_pH_sl'!$H$2:$H$7</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>org</t>
   </si>
@@ -166,12 +156,30 @@
   </si>
   <si>
     <t>sd_diff_slopes_buffer_enzym</t>
+  </si>
+  <si>
+    <t>pH10_buffer_1</t>
+  </si>
+  <si>
+    <t>pH10_buffer_2</t>
+  </si>
+  <si>
+    <t>pH10_buffer_3</t>
+  </si>
+  <si>
+    <t>pH10_p055_1</t>
+  </si>
+  <si>
+    <t>pH10_p055_2</t>
+  </si>
+  <si>
+    <t>pH10_p055_3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -731,10 +739,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.15854239885009358"/>
+          <c:x val="0.19561209526655593"/>
           <c:y val="2.6040104986876641E-2"/>
-          <c:w val="0.81114666835151128"/>
-          <c:h val="0.87121322834645665"/>
+          <c:w val="0.77407690543536445"/>
+          <c:h val="0.84598389077512104"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -772,10 +780,10 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'20230503_4NP_butyrate_p55_pH_sl'!$I$2:$I$7</c:f>
+                <c:f>'20230503_4NP_butyrate_p55_pH_sl'!$I$2:$I$8</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="6"/>
+                  <c:ptCount val="7"/>
                   <c:pt idx="0">
                     <c:v>5.8323161313464109E-5</c:v>
                   </c:pt>
@@ -794,15 +802,18 @@
                   <c:pt idx="5">
                     <c:v>5.6114056889032884E-4</c:v>
                   </c:pt>
+                  <c:pt idx="6">
+                    <c:v>4.9545419433539614E-2</c:v>
+                  </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'20230503_4NP_butyrate_p55_pH_sl'!$I$2:$I$7</c:f>
+                <c:f>'20230503_4NP_butyrate_p55_pH_sl'!$I$2:$I$8</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="6"/>
+                  <c:ptCount val="7"/>
                   <c:pt idx="0">
                     <c:v>5.8323161313464109E-5</c:v>
                   </c:pt>
@@ -820,6 +831,9 @@
                   </c:pt>
                   <c:pt idx="5">
                     <c:v>5.6114056889032884E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>4.9545419433539614E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -840,10 +854,10 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>'20230503_4NP_butyrate_p55_pH_sl'!$G$2:$G$7</c:f>
+              <c:f>'20230503_4NP_butyrate_p55_pH_sl'!$G$2:$G$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>6</c:v>
                 </c:pt>
@@ -862,15 +876,18 @@
                 <c:pt idx="5">
                   <c:v>9.5</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'20230503_4NP_butyrate_p55_pH_sl'!$H$2:$H$7</c:f>
+              <c:f>'20230503_4NP_butyrate_p55_pH_sl'!$H$2:$H$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2.3285714285714302E-2</c:v>
                 </c:pt>
@@ -888,6 +905,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.80605714285714014</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.43051428571428452</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1047,6 +1067,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="4.005637079455978E-2"/>
+              <c:y val="0.35836108502492237"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1730,15 +1758,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>679450</xdr:colOff>
+      <xdr:colOff>1168400</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>774700</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2062,11 +2090,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2202,11 +2230,11 @@
         <v>8.2285714285714202E-3</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" ref="C7:C37" si="0">SUM(B5:B7)</f>
+        <f t="shared" ref="C7:C43" si="0">SUM(B5:B7)</f>
         <v>2.4314285714285712E-2</v>
       </c>
       <c r="D7">
-        <f t="shared" ref="D7:D37" si="1">STDEV(B5:B7)</f>
+        <f t="shared" ref="D7:D43" si="1">STDEV(B5:B7)</f>
         <v>1.1547005383791315E-4</v>
       </c>
       <c r="E7" s="1">
@@ -2236,6 +2264,15 @@
       </c>
       <c r="C8" s="1"/>
       <c r="E8" s="1"/>
+      <c r="G8">
+        <v>10</v>
+      </c>
+      <c r="H8">
+        <v>0.43051428571428452</v>
+      </c>
+      <c r="I8">
+        <v>4.9545419433539614E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -2630,6 +2667,87 @@
       <c r="F37">
         <f t="shared" si="3"/>
         <v>5.6114056889032884E-4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38">
+        <v>8.9085714285714199E-2</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39">
+        <v>8.4942857142857195E-2</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40">
+        <v>9.1342857142857101E-2</v>
+      </c>
+      <c r="C40" s="1">
+        <f t="shared" ref="C38:C40" si="4">SUM(B38:B40)</f>
+        <v>0.26537142857142848</v>
+      </c>
+      <c r="D40">
+        <f t="shared" ref="D38:D40" si="5">STDEV(B38:B40)</f>
+        <v>3.2459708148120932E-3</v>
+      </c>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41">
+        <v>0.27722857142857099</v>
+      </c>
+      <c r="C41" s="1"/>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>46</v>
+      </c>
+      <c r="B42">
+        <v>0.24468571428571401</v>
+      </c>
+      <c r="C42" s="1"/>
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>47</v>
+      </c>
+      <c r="B43">
+        <v>0.173971428571428</v>
+      </c>
+      <c r="C43" s="1">
+        <f t="shared" si="0"/>
+        <v>0.695885714285713</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="1"/>
+        <v>5.2791390248351708E-2</v>
+      </c>
+      <c r="E43" s="1">
+        <f t="shared" ref="E38:E43" si="6">C43-C40</f>
+        <v>0.43051428571428452</v>
+      </c>
+      <c r="F43">
+        <f t="shared" ref="F38:F43" si="7">ABS(D43-D40)</f>
+        <v>4.9545419433539614E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>